<commit_message>
:white_check_mark: add tests for explicit typing in auto typing
</commit_message>
<xml_diff>
--- a/lutra-tab/src/test/resources/atomic/untypedLiterals.xlsx
+++ b/lutra-tab/src/test/resources/atomic/untypedLiterals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t xml:space="preserve">#OTTR</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t xml:space="preserve">!#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asdf^^xsd:normalizedString</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asdf^^ex:mydatatype</t>
   </si>
 </sst>
 </file>
@@ -186,16 +192,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:C16"/>
+  <dimension ref="A2:C18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -293,12 +298,22 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C18" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>